<commit_message>
Adding an Excel source - Day 46
</commit_message>
<xml_diff>
--- a/Source Files/Input01.xlsx
+++ b/Source Files/Input01.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\kjo1\SSIS-Practice\Source Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE948282-F55E-44C8-B0A4-E404CB57F842}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="14130" windowHeight="13808"/>
+    <workbookView xWindow="38400" yWindow="-1680" windowWidth="26850" windowHeight="20835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -236,6 +242,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -284,7 +293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,9 +326,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,6 +378,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -527,27 +570,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.06640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -605,7 +648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -634,7 +677,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -663,7 +706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -692,7 +735,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>12</v>
       </c>
@@ -721,7 +764,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
@@ -750,7 +793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>18</v>
       </c>
@@ -779,7 +822,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>19</v>
       </c>
@@ -814,24 +857,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>